<commit_message>
Update dataset - 2025-02-13 10:59:10
</commit_message>
<xml_diff>
--- a/datasets/methylation_lysine_exp.xlsx
+++ b/datasets/methylation_lysine_exp.xlsx
@@ -11265,7 +11265,7 @@
       </c>
       <c r="J226" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>me</t>
         </is>
       </c>
     </row>
@@ -11313,7 +11313,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>me</t>
         </is>
       </c>
     </row>
@@ -11553,7 +11553,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>me</t>
         </is>
       </c>
     </row>
@@ -11601,7 +11601,7 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>me</t>
         </is>
       </c>
     </row>
@@ -30921,7 +30921,7 @@
       </c>
       <c r="J639" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>me</t>
         </is>
       </c>
     </row>
@@ -30969,7 +30969,7 @@
       </c>
       <c r="J640" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>me</t>
         </is>
       </c>
     </row>
@@ -34823,7 +34823,7 @@
         </is>
       </c>
       <c r="E722" t="n">
-        <v>240</v>
+        <v>75</v>
       </c>
       <c r="F722" t="inlineStr">
         <is>
@@ -39685,7 +39685,7 @@
       </c>
       <c r="J823" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>me</t>
         </is>
       </c>
     </row>
@@ -39733,7 +39733,7 @@
       </c>
       <c r="J824" t="inlineStr">
         <is>
-          <t>m1</t>
+          <t>me</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update dataset - 2025-02-17 21:06:28
</commit_message>
<xml_diff>
--- a/datasets/methylation_lysine_exp.xlsx
+++ b/datasets/methylation_lysine_exp.xlsx
@@ -11265,7 +11265,7 @@
       </c>
       <c r="J226" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>m1-ac</t>
         </is>
       </c>
     </row>
@@ -11313,7 +11313,7 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>m1-ac</t>
         </is>
       </c>
     </row>
@@ -11553,7 +11553,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>m1-ac</t>
         </is>
       </c>
     </row>
@@ -11601,7 +11601,7 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>m1-ac</t>
         </is>
       </c>
     </row>
@@ -23525,7 +23525,7 @@
       </c>
       <c r="J483" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -23621,7 +23621,7 @@
       </c>
       <c r="J485" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -23717,7 +23717,7 @@
       </c>
       <c r="J487" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -23813,7 +23813,7 @@
       </c>
       <c r="J489" t="inlineStr">
         <is>
-          <t>m3</t>
+          <t>m3-OH</t>
         </is>
       </c>
     </row>
@@ -23861,7 +23861,7 @@
       </c>
       <c r="J490" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -23909,7 +23909,7 @@
       </c>
       <c r="J491" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -24005,7 +24005,7 @@
       </c>
       <c r="J493" t="inlineStr">
         <is>
-          <t>m3</t>
+          <t>m3-OH</t>
         </is>
       </c>
     </row>
@@ -24053,7 +24053,7 @@
       </c>
       <c r="J494" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -24101,7 +24101,7 @@
       </c>
       <c r="J495" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -24197,7 +24197,7 @@
       </c>
       <c r="J497" t="inlineStr">
         <is>
-          <t>m3</t>
+          <t>m3-OH</t>
         </is>
       </c>
     </row>
@@ -24245,7 +24245,7 @@
       </c>
       <c r="J498" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -24293,7 +24293,7 @@
       </c>
       <c r="J499" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -24389,7 +24389,7 @@
       </c>
       <c r="J501" t="inlineStr">
         <is>
-          <t>m3</t>
+          <t>m3-OH</t>
         </is>
       </c>
     </row>
@@ -24437,7 +24437,7 @@
       </c>
       <c r="J502" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -24485,7 +24485,7 @@
       </c>
       <c r="J503" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -24581,7 +24581,7 @@
       </c>
       <c r="J505" t="inlineStr">
         <is>
-          <t>m3</t>
+          <t>m3-OH</t>
         </is>
       </c>
     </row>
@@ -24629,7 +24629,7 @@
       </c>
       <c r="J506" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -30921,7 +30921,7 @@
       </c>
       <c r="J639" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>m1-ac</t>
         </is>
       </c>
     </row>
@@ -30969,7 +30969,7 @@
       </c>
       <c r="J640" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>m1-ac</t>
         </is>
       </c>
     </row>
@@ -36569,7 +36569,7 @@
       </c>
       <c r="J758" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>poly-mAP</t>
         </is>
       </c>
     </row>
@@ -39685,7 +39685,7 @@
       </c>
       <c r="J823" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>m1-ac</t>
         </is>
       </c>
     </row>
@@ -39733,7 +39733,7 @@
       </c>
       <c r="J824" t="inlineStr">
         <is>
-          <t>me</t>
+          <t>m1-ac</t>
         </is>
       </c>
     </row>

</xml_diff>